<commit_message>
Improve Telegram bot error handling and stability
Adds `nest_asyncio` to handle nested event loops, implements robust error handling for the Telegram bot with `try-except-finally` blocks, and includes graceful shutdown logic in `telegram_bot_enhanced.py`. Updates `requirements.txt` to include `nest-asyncio`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: 43fc148d-2011-45b6-b9da-aa84775f2a9c
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/376nkI8
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,36 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>5621813206</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Saad</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-11 11:05:59</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update user settings to reflect recent changes
No changes detected in the provided Git diff.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 4061fabe-21c1-4b29-ba35-2696e1d57c7a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/376nkI8
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-11 11:45:48</t>
+          <t>2025-11-11 11:50:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add images and update settings file to enhance user profiles
Add new image assets to the attached_assets directory and update the user_settings.xlsx file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 44d75496-df4b-43ab-aeac-316bb4ae1632
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/376nkI8
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-11 11:50:29</t>
+          <t>2025-11-11 11:51:44</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user settings for price change notifications
Modify user_settings.xlsx to include new fields for automated price change notifications.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 976299bd-a87d-4677-907e-845a3a2b221e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/376nkI8
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -479,7 +479,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-11 11:08:14</t>
+          <t>2025-11-11 12:44:02</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user settings spreadsheet to reflect current configurations
Updated the user_settings.xlsx file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 24f61adf-8032-4a60-a56c-fce1c27db1a9
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/Teo4A6H
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-11 21:14:35</t>
+          <t>2025-11-12 06:26:09</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new images and update user settings file
Added new image assets and updated the user_settings.xlsx file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 42b7a2d3-9c6c-4eed-b862-8e302ffb5ed0
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/Llwyc9Q
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -494,12 +494,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ar</t>
+          <t>en</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-12 06:26:09</t>
+          <t>2025-11-12 06:55:37</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Saved progress after completing a task
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: 7f2a9979-4c88-458e-86e1-60f24dba6834
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/Llwyc9Q
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,16 @@
           <t>Last Updated</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Last Activity</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Last Welcome</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -480,6 +490,11 @@
       <c r="F2" t="inlineStr">
         <is>
           <t>2025-11-11 12:44:02</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-12 07:46:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enable settings for user preferences and configurations
Update user settings to enable new preference options.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: a3c9f166-c2ae-4c6d-a46a-984e048edd6a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/Llwyc9Q
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -514,7 +514,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -524,7 +524,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-12 06:55:37</t>
+          <t>2025-11-12 09:06:47</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user settings to reflect project management changes
Updated user_settings.xlsx to reflect changes in project roles and responsibilities.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: e6a61fdd-e6cf-4323-9c99-ad4c05fcdf8c
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/Llwyc9Q
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -489,7 +489,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-11 12:44:02</t>
+          <t>2025-11-12 09:48:39</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">

</xml_diff>

<commit_message>
Enhance bot to provide instant price change alerts and summary reports
Modify `EnhancedTelegramBot` to check prices 60 times per minute for instant alerts, introduce a 2-hour summary report, and update the web interface with a control panel and API endpoints for bot statistics and testing. Default auto-signals to true for all users in `UserStorage`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 90b24820-2d7c-494d-9924-def783cf1de4
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/RCYpEyh
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -489,7 +489,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-12 09:48:39</t>
+          <t>2025-11-12 10:32:15</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -524,7 +524,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-12 09:06:47</t>
+          <t>2025-11-12 10:32:15</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user settings to reflect recent market analysis
Updated user_settings.xlsx to adjust parameters based on recent market analysis, incorporating small percentage differences observed over a 30-second period.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 2f474f9f-5f30-4c6f-baa2-6fc158eca29f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/RCYpEyh
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -537,6 +537,11 @@
           <t>2025-11-12 11:08:05</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-11-12 12:10:43</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add clickable links to currency prices and lower alert sensitivity
Update the bot to provide direct links to Binance market pages for currencies and decrease the price change threshold for alerts to 0.1% to catch smaller fluctuations.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: e40d3159-304b-441e-9452-882765da61a8
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/RCYpEyh
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -529,17 +529,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-12 11:07:50</t>
+          <t>2025-11-12 12:19:07</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-12 11:08:05</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2025-11-12 12:10:43</t>
+          <t>2025-11-12 12:20:14</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user settings file
No changes detected in the provided diff.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 216bdc86-2067-4518-9c5b-291d42f881f0
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/RCYpEyh
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -537,6 +537,11 @@
           <t>2025-11-12 12:20:14</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-11-12 13:22:34</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update user settings spreadsheet with new information
Updated user_settings.xlsx file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 93bcd462-d495-43ae-8312-23f540c0645e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/RCYpEyh
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -514,7 +514,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ar</t>
+          <t>en</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -529,17 +529,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-12 12:19:07</t>
+          <t>2025-11-12 14:20:26</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-12 12:20:14</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2025-11-12 13:22:34</t>
+          <t>2025-11-12 14:20:36</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Transitioned from Plan to Build mode
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: ff54e208-dec4-4daa-a828-f7ae0a06ed23
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/RCYpEyh
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-11-12 13:42:34</t>
+          <t>2025-11-12 14:47:36</t>
         </is>
       </c>
     </row>
@@ -535,6 +535,11 @@
       <c r="G3" t="inlineStr">
         <is>
           <t>2025-11-12 14:20:36</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-11-12 15:27:35</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user settings to reflect the latest configurations
No changes were detected in the provided diff.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 1edf138e-1616-42e3-a1d3-84109371e23e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/ocIpsuu
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-11-12 18:06:31</t>
+          <t>2025-11-12 19:06:51</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-11-12 17:36:31</t>
+          <t>2025-11-12 18:46:51</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user settings spreadsheet
No changes made to user_settings.xlsx.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 330278cd-2dbd-48ee-807d-5148c32aa091
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/ocIpsuu
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-11-12 19:06:51</t>
+          <t>2025-11-12 20:16:51</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-11-12 18:46:51</t>
+          <t>2025-11-12 19:56:51</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update settings for all available tools
Updates the user settings for all tools, impacting the user_settings.xlsx file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 6162a9a9-5d2e-44ec-9cba-07f11c5e2212
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/CleSy5A
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-11-12 20:16:51</t>
+          <t>2025-11-13 02:10:02</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-11-12 19:56:51</t>
+          <t>2025-11-13 02:10:02</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user settings and add an attached image asset
Updated user_settings.xlsx and added attached_assets/image_1763017020651.png.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 8ee1159d-cd72-4ced-9dbc-4e857c08228a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/CleSy5A
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-11-13 02:10:02</t>
+          <t>2025-11-13 06:25:35</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-11-13 02:10:02</t>
+          <t>2025-11-13 06:25:35</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update settings for user profiles
No changes were made to the user_settings.xlsx file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: eaa775eb-ab7e-47ea-beb9-851f8fbbb0cc
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/53d93ca0-c4ee-48fc-977b-52aee7a8a365/4bc880fa-4b8e-4b3a-9798-bfb3ab20ba80/CleSy5A
</commit_message>
<xml_diff>
--- a/user_settings.xlsx
+++ b/user_settings.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-11-13 06:25:35</t>
+          <t>2025-11-13 09:55:35</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-11-13 06:25:35</t>
+          <t>2025-11-13 09:55:36</t>
         </is>
       </c>
     </row>

</xml_diff>